<commit_message>
MOD data without inf values
</commit_message>
<xml_diff>
--- a/data/inventory_data_new.xlsx
+++ b/data/inventory_data_new.xlsx
@@ -877,9 +877,13 @@
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>100</v>
+      </c>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="K8" t="n">
+        <v>100</v>
+      </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
@@ -947,9 +951,13 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>100</v>
+      </c>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="n">
+        <v>100</v>
+      </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" s="2" t="n">
@@ -1365,9 +1373,13 @@
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>100</v>
+      </c>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>100</v>
+      </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" s="2" t="n">
@@ -2567,9 +2579,13 @@
       <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>100</v>
+      </c>
       <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
+      <c r="K42" t="n">
+        <v>100</v>
+      </c>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
@@ -3075,9 +3091,13 @@
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
+      <c r="I54" t="n">
+        <v>100</v>
+      </c>
       <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr"/>
+      <c r="K54" t="n">
+        <v>100</v>
+      </c>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
       <c r="N54" s="2" t="n">
@@ -3261,9 +3281,13 @@
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
+      <c r="I58" t="n">
+        <v>100</v>
+      </c>
       <c r="J58" t="inlineStr"/>
-      <c r="K58" t="inlineStr"/>
+      <c r="K58" t="n">
+        <v>100</v>
+      </c>
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="inlineStr"/>
@@ -3838,9 +3862,13 @@
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
+      <c r="I69" t="n">
+        <v>100</v>
+      </c>
       <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
+      <c r="K69" t="n">
+        <v>100</v>
+      </c>
       <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
       <c r="N69" s="2" t="n">
@@ -4124,9 +4152,13 @@
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
+      <c r="I75" t="n">
+        <v>100</v>
+      </c>
       <c r="J75" t="inlineStr"/>
-      <c r="K75" t="inlineStr"/>
+      <c r="K75" t="n">
+        <v>100</v>
+      </c>
       <c r="L75" t="inlineStr"/>
       <c r="M75" t="inlineStr"/>
       <c r="N75" s="2" t="n">
@@ -5406,11 +5438,15 @@
       <c r="H97" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr"/>
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
       <c r="J97" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr"/>
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
       <c r="L97" t="inlineStr"/>
       <c r="M97" t="inlineStr"/>
       <c r="N97" s="2" t="n">
@@ -6148,9 +6184,13 @@
       <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="inlineStr"/>
-      <c r="I111" t="inlineStr"/>
+      <c r="I111" t="n">
+        <v>100</v>
+      </c>
       <c r="J111" t="inlineStr"/>
-      <c r="K111" t="inlineStr"/>
+      <c r="K111" t="n">
+        <v>100</v>
+      </c>
       <c r="L111" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
       <c r="N111" t="inlineStr"/>
@@ -7754,9 +7794,13 @@
       <c r="F141" t="inlineStr"/>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="inlineStr"/>
-      <c r="I141" t="inlineStr"/>
+      <c r="I141" t="n">
+        <v>100</v>
+      </c>
       <c r="J141" t="inlineStr"/>
-      <c r="K141" t="inlineStr"/>
+      <c r="K141" t="n">
+        <v>100</v>
+      </c>
       <c r="L141" t="inlineStr"/>
       <c r="M141" t="inlineStr"/>
       <c r="N141" s="2" t="n">
@@ -10407,9 +10451,13 @@
       <c r="F192" t="inlineStr"/>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="inlineStr"/>
-      <c r="I192" t="inlineStr"/>
+      <c r="I192" t="n">
+        <v>100</v>
+      </c>
       <c r="J192" t="inlineStr"/>
-      <c r="K192" t="inlineStr"/>
+      <c r="K192" t="n">
+        <v>100</v>
+      </c>
       <c r="L192" t="inlineStr"/>
       <c r="M192" t="inlineStr"/>
       <c r="N192" s="2" t="n">
@@ -10540,9 +10588,13 @@
       <c r="F195" t="inlineStr"/>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="inlineStr"/>
-      <c r="I195" t="inlineStr"/>
+      <c r="I195" t="n">
+        <v>100</v>
+      </c>
       <c r="J195" t="inlineStr"/>
-      <c r="K195" t="inlineStr"/>
+      <c r="K195" t="n">
+        <v>100</v>
+      </c>
       <c r="L195" t="inlineStr"/>
       <c r="M195" t="inlineStr"/>
       <c r="N195" s="2" t="n">
@@ -11747,18 +11799,14 @@
       <c r="H218" t="n">
         <v>24000</v>
       </c>
-      <c r="I218" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I218" t="n">
+        <v>100</v>
       </c>
       <c r="J218" t="n">
         <v>1664.88</v>
       </c>
-      <c r="K218" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K218" t="n">
+        <v>100</v>
       </c>
       <c r="L218" t="inlineStr"/>
       <c r="M218" t="inlineStr"/>
@@ -13211,18 +13259,14 @@
       <c r="H248" t="n">
         <v>96000</v>
       </c>
-      <c r="I248" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I248" t="n">
+        <v>100</v>
       </c>
       <c r="J248" t="n">
         <v>24744.5</v>
       </c>
-      <c r="K248" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K248" t="n">
+        <v>100</v>
       </c>
       <c r="L248" t="inlineStr"/>
       <c r="M248" t="inlineStr"/>
@@ -13425,9 +13469,13 @@
       <c r="F252" t="inlineStr"/>
       <c r="G252" t="inlineStr"/>
       <c r="H252" t="inlineStr"/>
-      <c r="I252" t="inlineStr"/>
+      <c r="I252" t="n">
+        <v>100</v>
+      </c>
       <c r="J252" t="inlineStr"/>
-      <c r="K252" t="inlineStr"/>
+      <c r="K252" t="n">
+        <v>100</v>
+      </c>
       <c r="L252" t="inlineStr"/>
       <c r="M252" t="inlineStr"/>
       <c r="N252" s="2" t="n">
@@ -15173,9 +15221,13 @@
       <c r="F284" t="inlineStr"/>
       <c r="G284" t="inlineStr"/>
       <c r="H284" t="inlineStr"/>
-      <c r="I284" t="inlineStr"/>
+      <c r="I284" t="n">
+        <v>100</v>
+      </c>
       <c r="J284" t="inlineStr"/>
-      <c r="K284" t="inlineStr"/>
+      <c r="K284" t="n">
+        <v>100</v>
+      </c>
       <c r="L284" t="inlineStr"/>
       <c r="M284" t="inlineStr"/>
       <c r="N284" t="inlineStr"/>
@@ -15332,11 +15384,15 @@
       <c r="H287" t="n">
         <v>0</v>
       </c>
-      <c r="I287" t="inlineStr"/>
+      <c r="I287" t="n">
+        <v>0</v>
+      </c>
       <c r="J287" t="n">
         <v>0</v>
       </c>
-      <c r="K287" t="inlineStr"/>
+      <c r="K287" t="n">
+        <v>0</v>
+      </c>
       <c r="L287" t="inlineStr"/>
       <c r="M287" t="inlineStr"/>
       <c r="N287" s="2" t="n">
@@ -15897,9 +15953,13 @@
       <c r="F298" t="inlineStr"/>
       <c r="G298" t="inlineStr"/>
       <c r="H298" t="inlineStr"/>
-      <c r="I298" t="inlineStr"/>
+      <c r="I298" t="n">
+        <v>100</v>
+      </c>
       <c r="J298" t="inlineStr"/>
-      <c r="K298" t="inlineStr"/>
+      <c r="K298" t="n">
+        <v>100</v>
+      </c>
       <c r="L298" t="inlineStr"/>
       <c r="M298" t="inlineStr"/>
       <c r="N298" t="inlineStr"/>
@@ -16474,9 +16534,13 @@
       <c r="F309" t="inlineStr"/>
       <c r="G309" t="inlineStr"/>
       <c r="H309" t="inlineStr"/>
-      <c r="I309" t="inlineStr"/>
+      <c r="I309" t="n">
+        <v>100</v>
+      </c>
       <c r="J309" t="inlineStr"/>
-      <c r="K309" t="inlineStr"/>
+      <c r="K309" t="n">
+        <v>100</v>
+      </c>
       <c r="L309" t="inlineStr"/>
       <c r="M309" t="inlineStr"/>
       <c r="N309" s="2" t="n">
@@ -17233,18 +17297,14 @@
       <c r="H324" t="n">
         <v>274450</v>
       </c>
-      <c r="I324" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I324" t="n">
+        <v>100</v>
       </c>
       <c r="J324" t="n">
         <v>36995.86</v>
       </c>
-      <c r="K324" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K324" t="n">
+        <v>100</v>
       </c>
       <c r="L324" t="inlineStr"/>
       <c r="M324" t="inlineStr"/>
@@ -17290,18 +17350,14 @@
       <c r="H325" t="n">
         <v>208450</v>
       </c>
-      <c r="I325" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I325" t="n">
+        <v>100</v>
       </c>
       <c r="J325" t="n">
         <v>40650.11</v>
       </c>
-      <c r="K325" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K325" t="n">
+        <v>100</v>
       </c>
       <c r="L325" t="inlineStr"/>
       <c r="M325" t="inlineStr"/>
@@ -19551,9 +19607,13 @@
       <c r="F370" t="inlineStr"/>
       <c r="G370" t="inlineStr"/>
       <c r="H370" t="inlineStr"/>
-      <c r="I370" t="inlineStr"/>
+      <c r="I370" t="n">
+        <v>100</v>
+      </c>
       <c r="J370" t="inlineStr"/>
-      <c r="K370" t="inlineStr"/>
+      <c r="K370" t="n">
+        <v>100</v>
+      </c>
       <c r="L370" t="inlineStr"/>
       <c r="M370" t="inlineStr"/>
       <c r="N370" t="inlineStr"/>
@@ -30088,18 +30148,14 @@
       <c r="H573" t="n">
         <v>2886400</v>
       </c>
-      <c r="I573" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I573" t="n">
+        <v>100</v>
       </c>
       <c r="J573" t="n">
         <v>107762.97</v>
       </c>
-      <c r="K573" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K573" t="n">
+        <v>100</v>
       </c>
       <c r="L573" t="inlineStr"/>
       <c r="M573" t="inlineStr"/>
@@ -30145,18 +30201,14 @@
       <c r="H574" t="n">
         <v>2395800</v>
       </c>
-      <c r="I574" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I574" t="n">
+        <v>100</v>
       </c>
       <c r="J574" t="n">
         <v>93333.33</v>
       </c>
-      <c r="K574" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K574" t="n">
+        <v>100</v>
       </c>
       <c r="L574" t="inlineStr"/>
       <c r="M574" t="inlineStr"/>
@@ -30794,9 +30846,13 @@
       <c r="F587" t="inlineStr"/>
       <c r="G587" t="inlineStr"/>
       <c r="H587" t="inlineStr"/>
-      <c r="I587" t="inlineStr"/>
+      <c r="I587" t="n">
+        <v>100</v>
+      </c>
       <c r="J587" t="inlineStr"/>
-      <c r="K587" t="inlineStr"/>
+      <c r="K587" t="n">
+        <v>100</v>
+      </c>
       <c r="L587" t="inlineStr"/>
       <c r="M587" t="inlineStr"/>
       <c r="N587" s="2" t="n">
@@ -31622,9 +31678,13 @@
       <c r="F603" t="inlineStr"/>
       <c r="G603" t="inlineStr"/>
       <c r="H603" t="inlineStr"/>
-      <c r="I603" t="inlineStr"/>
+      <c r="I603" t="n">
+        <v>100</v>
+      </c>
       <c r="J603" t="inlineStr"/>
-      <c r="K603" t="inlineStr"/>
+      <c r="K603" t="n">
+        <v>100</v>
+      </c>
       <c r="L603" t="inlineStr"/>
       <c r="M603" t="inlineStr"/>
       <c r="N603" t="inlineStr"/>
@@ -31899,9 +31959,13 @@
       <c r="F608" t="inlineStr"/>
       <c r="G608" t="inlineStr"/>
       <c r="H608" t="inlineStr"/>
-      <c r="I608" t="inlineStr"/>
+      <c r="I608" t="n">
+        <v>100</v>
+      </c>
       <c r="J608" t="inlineStr"/>
-      <c r="K608" t="inlineStr"/>
+      <c r="K608" t="n">
+        <v>100</v>
+      </c>
       <c r="L608" t="inlineStr"/>
       <c r="M608" t="inlineStr"/>
       <c r="N608" s="2" t="n">
@@ -35274,9 +35338,13 @@
       <c r="F669" t="inlineStr"/>
       <c r="G669" t="inlineStr"/>
       <c r="H669" t="inlineStr"/>
-      <c r="I669" t="inlineStr"/>
+      <c r="I669" t="n">
+        <v>100</v>
+      </c>
       <c r="J669" t="inlineStr"/>
-      <c r="K669" t="inlineStr"/>
+      <c r="K669" t="n">
+        <v>100</v>
+      </c>
       <c r="L669" t="inlineStr"/>
       <c r="M669" t="inlineStr"/>
       <c r="N669" t="inlineStr"/>
@@ -37812,9 +37880,13 @@
       <c r="F727" t="inlineStr"/>
       <c r="G727" t="inlineStr"/>
       <c r="H727" t="inlineStr"/>
-      <c r="I727" t="inlineStr"/>
+      <c r="I727" t="n">
+        <v>100</v>
+      </c>
       <c r="J727" t="inlineStr"/>
-      <c r="K727" t="inlineStr"/>
+      <c r="K727" t="n">
+        <v>100</v>
+      </c>
       <c r="L727" t="inlineStr"/>
       <c r="M727" t="inlineStr"/>
       <c r="N727" t="inlineStr"/>
@@ -38134,9 +38206,13 @@
       <c r="F735" t="inlineStr"/>
       <c r="G735" t="inlineStr"/>
       <c r="H735" t="inlineStr"/>
-      <c r="I735" t="inlineStr"/>
+      <c r="I735" t="n">
+        <v>100</v>
+      </c>
       <c r="J735" t="inlineStr"/>
-      <c r="K735" t="inlineStr"/>
+      <c r="K735" t="n">
+        <v>100</v>
+      </c>
       <c r="L735" t="inlineStr"/>
       <c r="M735" t="inlineStr"/>
       <c r="N735" t="inlineStr"/>
@@ -38793,18 +38869,14 @@
       <c r="H750" t="n">
         <v>69686400</v>
       </c>
-      <c r="I750" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I750" t="n">
+        <v>100</v>
       </c>
       <c r="J750" t="n">
         <v>327748.05</v>
       </c>
-      <c r="K750" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K750" t="n">
+        <v>100</v>
       </c>
       <c r="L750" t="inlineStr"/>
       <c r="M750" t="inlineStr"/>
@@ -39955,11 +40027,15 @@
       <c r="H772" t="n">
         <v>0</v>
       </c>
-      <c r="I772" t="inlineStr"/>
+      <c r="I772" t="n">
+        <v>0</v>
+      </c>
       <c r="J772" t="n">
         <v>0</v>
       </c>
-      <c r="K772" t="inlineStr"/>
+      <c r="K772" t="n">
+        <v>0</v>
+      </c>
       <c r="L772" t="inlineStr"/>
       <c r="M772" t="inlineStr"/>
       <c r="N772" s="2" t="n">
@@ -41146,18 +41222,14 @@
       <c r="H795" t="n">
         <v>78244000</v>
       </c>
-      <c r="I795" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I795" t="n">
+        <v>100</v>
       </c>
       <c r="J795" t="n">
         <v>435020.83</v>
       </c>
-      <c r="K795" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K795" t="n">
+        <v>100</v>
       </c>
       <c r="L795" t="inlineStr"/>
       <c r="M795" t="inlineStr"/>
@@ -41564,9 +41636,13 @@
       <c r="F805" t="inlineStr"/>
       <c r="G805" t="inlineStr"/>
       <c r="H805" t="inlineStr"/>
-      <c r="I805" t="inlineStr"/>
+      <c r="I805" t="n">
+        <v>100</v>
+      </c>
       <c r="J805" t="inlineStr"/>
-      <c r="K805" t="inlineStr"/>
+      <c r="K805" t="n">
+        <v>100</v>
+      </c>
       <c r="L805" t="inlineStr"/>
       <c r="M805" t="inlineStr"/>
       <c r="N805" t="inlineStr"/>
@@ -41599,11 +41675,15 @@
       <c r="H806" t="n">
         <v>0</v>
       </c>
-      <c r="I806" t="inlineStr"/>
+      <c r="I806" t="n">
+        <v>0</v>
+      </c>
       <c r="J806" t="n">
         <v>0</v>
       </c>
-      <c r="K806" t="inlineStr"/>
+      <c r="K806" t="n">
+        <v>0</v>
+      </c>
       <c r="L806" t="inlineStr"/>
       <c r="M806" t="inlineStr"/>
       <c r="N806" t="inlineStr"/>
@@ -41992,9 +42072,13 @@
       <c r="F815" t="inlineStr"/>
       <c r="G815" t="inlineStr"/>
       <c r="H815" t="inlineStr"/>
-      <c r="I815" t="inlineStr"/>
+      <c r="I815" t="n">
+        <v>100</v>
+      </c>
       <c r="J815" t="inlineStr"/>
-      <c r="K815" t="inlineStr"/>
+      <c r="K815" t="n">
+        <v>100</v>
+      </c>
       <c r="L815" t="inlineStr"/>
       <c r="M815" t="inlineStr"/>
       <c r="N815" t="inlineStr"/>
@@ -42846,9 +42930,13 @@
       <c r="F831" t="inlineStr"/>
       <c r="G831" t="inlineStr"/>
       <c r="H831" t="inlineStr"/>
-      <c r="I831" t="inlineStr"/>
+      <c r="I831" t="n">
+        <v>100</v>
+      </c>
       <c r="J831" t="inlineStr"/>
-      <c r="K831" t="inlineStr"/>
+      <c r="K831" t="n">
+        <v>100</v>
+      </c>
       <c r="L831" t="inlineStr"/>
       <c r="M831" t="inlineStr"/>
       <c r="N831" s="2" t="n">
@@ -45198,9 +45286,13 @@
       <c r="F871" t="inlineStr"/>
       <c r="G871" t="inlineStr"/>
       <c r="H871" t="inlineStr"/>
-      <c r="I871" t="inlineStr"/>
+      <c r="I871" t="n">
+        <v>100</v>
+      </c>
       <c r="J871" t="inlineStr"/>
-      <c r="K871" t="inlineStr"/>
+      <c r="K871" t="n">
+        <v>100</v>
+      </c>
       <c r="L871" t="inlineStr"/>
       <c r="M871" t="inlineStr"/>
       <c r="N871" t="inlineStr"/>
@@ -48269,9 +48361,13 @@
       <c r="F942" t="inlineStr"/>
       <c r="G942" t="inlineStr"/>
       <c r="H942" t="inlineStr"/>
-      <c r="I942" t="inlineStr"/>
+      <c r="I942" t="n">
+        <v>100</v>
+      </c>
       <c r="J942" t="inlineStr"/>
-      <c r="K942" t="inlineStr"/>
+      <c r="K942" t="n">
+        <v>100</v>
+      </c>
       <c r="L942" t="inlineStr"/>
       <c r="M942" t="inlineStr"/>
       <c r="N942" s="2" t="n">
@@ -49029,18 +49125,14 @@
       <c r="H956" t="n">
         <v>3960000</v>
       </c>
-      <c r="I956" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I956" t="n">
+        <v>100</v>
       </c>
       <c r="J956" t="n">
         <v>27434.88</v>
       </c>
-      <c r="K956" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K956" t="n">
+        <v>100</v>
       </c>
       <c r="L956" t="inlineStr"/>
       <c r="M956" t="inlineStr"/>
@@ -50232,18 +50324,14 @@
       <c r="H977" t="n">
         <v>19200</v>
       </c>
-      <c r="I977" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I977" t="n">
+        <v>100</v>
       </c>
       <c r="J977" t="n">
         <v>4669.44</v>
       </c>
-      <c r="K977" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="K977" t="n">
+        <v>100</v>
       </c>
       <c r="L977" t="inlineStr"/>
       <c r="M977" t="inlineStr"/>
@@ -50759,9 +50847,13 @@
       <c r="F986" t="inlineStr"/>
       <c r="G986" t="inlineStr"/>
       <c r="H986" t="inlineStr"/>
-      <c r="I986" t="inlineStr"/>
+      <c r="I986" t="n">
+        <v>100</v>
+      </c>
       <c r="J986" t="inlineStr"/>
-      <c r="K986" t="inlineStr"/>
+      <c r="K986" t="n">
+        <v>100</v>
+      </c>
       <c r="L986" t="inlineStr"/>
       <c r="M986" t="inlineStr"/>
       <c r="N986" s="2" t="n">
@@ -51964,9 +52056,13 @@
       <c r="F1007" t="inlineStr"/>
       <c r="G1007" t="inlineStr"/>
       <c r="H1007" t="inlineStr"/>
-      <c r="I1007" t="inlineStr"/>
+      <c r="I1007" t="n">
+        <v>100</v>
+      </c>
       <c r="J1007" t="inlineStr"/>
-      <c r="K1007" t="inlineStr"/>
+      <c r="K1007" t="n">
+        <v>100</v>
+      </c>
       <c r="L1007" t="inlineStr"/>
       <c r="M1007" t="inlineStr"/>
       <c r="N1007" t="inlineStr"/>

</xml_diff>